<commit_message>
README added; algorithm execution sequence changed, benchmark test results updated
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub.kolada\Documents\go_sudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1653AB8E-6862-494F-8E4D-BC0EEFFF56A9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BBB4F1-F5EA-42C8-B57A-E26183CC86FD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{666A6699-6131-4AB1-A29E-7DACA2D9F716}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="18">
   <si>
     <t>Sudoku level</t>
   </si>
@@ -71,16 +71,10 @@
     <t>Backtracking by block [ns]</t>
   </si>
   <si>
-    <t>Conclusion:</t>
-  </si>
-  <si>
     <t>must improve block backtracking algorithm</t>
   </si>
   <si>
     <t>must implement another deduction algorithms (x-cycles and swordfish)</t>
-  </si>
-  <si>
-    <t>Deduction algorithms do have better efficiency with solving sudokus, especially the harder ones</t>
   </si>
   <si>
     <t>Comparison</t>
@@ -221,9 +215,13 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -233,13 +231,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7BD8A7-F08D-41BA-B080-BFE118E322A3}">
   <dimension ref="A5:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,102 +571,103 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="G5" s="11" t="s">
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="G5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11" t="s">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="19"/>
+      <c r="E6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11" t="s">
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11" t="s">
+      <c r="J6" s="19"/>
+      <c r="K6" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="E7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
       <c r="I7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="11"/>
+      <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>4627</v>
+        <v>7380</v>
       </c>
       <c r="D8" s="1">
-        <v>5633</v>
+        <v>8819</v>
       </c>
       <c r="E8" s="1">
-        <v>19888</v>
+        <v>11198</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H8" s="1">
+        <f>B8</f>
         <v>1</v>
       </c>
       <c r="I8" s="5">
         <f>C8/1000000000</f>
-        <v>4.6269999999999999E-6</v>
+        <v>7.3799999999999996E-6</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" ref="J8:K18" si="0">D8/1000000000</f>
-        <v>5.6330000000000001E-6</v>
+        <v>8.8189999999999998E-6</v>
       </c>
       <c r="K8" s="6">
         <f t="shared" si="0"/>
-        <v>1.9888E-5</v>
+        <v>1.1198E-5</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -683,23 +678,24 @@
         <v>2</v>
       </c>
       <c r="C9" s="1">
-        <v>393779</v>
+        <v>382383</v>
       </c>
       <c r="D9" s="1">
         <v>607143</v>
       </c>
       <c r="E9" s="1">
-        <v>32261</v>
+        <v>17909</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="1">
+        <f t="shared" ref="H9:H18" si="1">B9</f>
         <v>2</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" ref="I9:I18" si="1">C9/1000000000</f>
-        <v>3.9377900000000003E-4</v>
+        <f t="shared" ref="I9:I18" si="2">C9/1000000000</f>
+        <v>3.8238299999999997E-4</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="0"/>
@@ -707,7 +703,7 @@
       </c>
       <c r="K9" s="5">
         <f t="shared" si="0"/>
-        <v>3.2261000000000002E-5</v>
+        <v>1.7909000000000001E-5</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -724,16 +720,17 @@
         <v>221174</v>
       </c>
       <c r="E10" s="1">
-        <v>74457</v>
+        <v>37858</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H10" s="1">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6130699999999999E-4</v>
       </c>
       <c r="J10" s="4">
@@ -742,7 +739,7 @@
       </c>
       <c r="K10" s="5">
         <f t="shared" si="0"/>
-        <v>7.4456999999999995E-5</v>
+        <v>3.7858000000000002E-5</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -753,31 +750,32 @@
         <v>4</v>
       </c>
       <c r="C11" s="1">
-        <v>675112</v>
+        <v>632639</v>
       </c>
       <c r="D11" s="1">
-        <v>807543</v>
-      </c>
-      <c r="E11" s="15">
-        <v>119632</v>
+        <v>798050</v>
+      </c>
+      <c r="E11" s="11">
+        <v>106140</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H11" s="1">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="1"/>
-        <v>6.7511199999999996E-4</v>
+        <f t="shared" si="2"/>
+        <v>6.3263900000000005E-4</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="0"/>
-        <v>8.0754299999999998E-4</v>
+        <v>7.9805000000000002E-4</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="0"/>
-        <v>1.19632E-4</v>
+        <v>1.0614E-4</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -788,31 +786,32 @@
         <v>5</v>
       </c>
       <c r="C12" s="1">
-        <v>276664</v>
+        <v>275644</v>
       </c>
       <c r="D12" s="1">
-        <v>311020</v>
+        <v>306227</v>
       </c>
       <c r="E12" s="1">
-        <v>93447</v>
+        <v>81753</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H12" s="1">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="1"/>
-        <v>2.7666399999999998E-4</v>
+        <f t="shared" si="2"/>
+        <v>2.7564400000000002E-4</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="0"/>
-        <v>3.1102000000000001E-4</v>
+        <v>3.0622700000000001E-4</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="0"/>
-        <v>9.3447000000000002E-5</v>
+        <v>8.1753000000000001E-5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -823,31 +822,32 @@
         <v>6</v>
       </c>
       <c r="C13" s="1">
-        <v>359794</v>
+        <v>360593</v>
       </c>
       <c r="D13" s="1">
-        <v>215476</v>
+        <v>216975</v>
       </c>
       <c r="E13" s="1">
-        <v>118332</v>
+        <v>138219</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H13" s="1">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="1"/>
-        <v>3.5979399999999998E-4</v>
+        <f t="shared" si="2"/>
+        <v>3.6059299999999998E-4</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="0"/>
-        <v>2.1547600000000001E-4</v>
+        <v>2.16975E-4</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="0"/>
-        <v>1.18332E-4</v>
+        <v>1.38219E-4</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -858,31 +858,32 @@
         <v>7</v>
       </c>
       <c r="C14" s="1">
-        <v>5926595</v>
+        <v>5796629</v>
       </c>
       <c r="D14" s="1">
-        <v>9234762</v>
+        <v>9114752</v>
       </c>
       <c r="E14" s="1">
-        <v>77706</v>
+        <v>80804</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H14" s="1">
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="1"/>
-        <v>5.9265949999999998E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.7966290000000002E-3</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="0"/>
-        <v>9.2347620000000005E-3</v>
+        <v>9.1147520000000003E-3</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="0"/>
-        <v>7.7706000000000004E-5</v>
+        <v>8.0803999999999994E-5</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -893,10 +894,10 @@
         <v>8</v>
       </c>
       <c r="C15" s="1">
-        <v>87899565</v>
+        <v>86150620</v>
       </c>
       <c r="D15" s="1">
-        <v>48038473</v>
+        <v>47439333</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>10</v>
@@ -905,15 +906,16 @@
         <v>4</v>
       </c>
       <c r="H15" s="1">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="1"/>
-        <v>8.7899564999999999E-2</v>
+        <f t="shared" si="2"/>
+        <v>8.6150619999999997E-2</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="0"/>
-        <v>4.8038472999999998E-2</v>
+        <v>4.7439333E-2</v>
       </c>
       <c r="K15" s="9" t="s">
         <v>10</v>
@@ -927,10 +929,10 @@
         <v>9</v>
       </c>
       <c r="C16" s="1">
-        <v>3368096</v>
+        <v>3336116</v>
       </c>
       <c r="D16" s="1">
-        <v>1288275</v>
+        <v>1257266</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>10</v>
@@ -939,15 +941,16 @@
         <v>4</v>
       </c>
       <c r="H16" s="1">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" si="1"/>
-        <v>3.3680960000000001E-3</v>
+        <f t="shared" si="2"/>
+        <v>3.3361160000000001E-3</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" si="0"/>
-        <v>1.288275E-3</v>
+        <v>1.2572659999999999E-3</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>10</v>
@@ -961,10 +964,10 @@
         <v>10</v>
       </c>
       <c r="C17" s="1">
-        <v>2116785</v>
+        <v>2097809</v>
       </c>
       <c r="D17" s="1">
-        <v>1632063</v>
+        <v>1611088</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>10</v>
@@ -973,15 +976,16 @@
         <v>4</v>
       </c>
       <c r="H17" s="1">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I17" s="4">
-        <f t="shared" si="1"/>
-        <v>2.1167849999999999E-3</v>
+        <f t="shared" si="2"/>
+        <v>2.097809E-3</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="0"/>
-        <v>1.632063E-3</v>
+        <v>1.6110880000000001E-3</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>10</v>
@@ -995,10 +999,10 @@
         <v>11</v>
       </c>
       <c r="C18" s="1">
-        <v>8030464</v>
+        <v>7955443</v>
       </c>
       <c r="D18" s="1">
-        <v>19278927</v>
+        <v>19118997</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>10</v>
@@ -1007,185 +1011,186 @@
         <v>5</v>
       </c>
       <c r="H18" s="1">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="I18" s="4">
-        <f t="shared" si="1"/>
-        <v>8.0304639999999993E-3</v>
+        <f t="shared" si="2"/>
+        <v>7.9554429999999995E-3</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" si="0"/>
-        <v>1.9278927000000001E-2</v>
+        <v>1.9118996999999999E-2</v>
       </c>
       <c r="K18" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
-      <c r="H20" s="12" t="s">
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
+      <c r="H20" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="14"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="18"/>
       <c r="L20" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" ref="C21:E22" si="2">AVERAGE(C8)</f>
-        <v>4627</v>
+        <f t="shared" ref="C21:E22" si="3">AVERAGE(C8)</f>
+        <v>7380</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="2"/>
-        <v>5633</v>
+        <f t="shared" si="3"/>
+        <v>8819</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="2"/>
-        <v>19888</v>
+        <f t="shared" si="3"/>
+        <v>11198</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I21" s="8">
-        <f t="shared" ref="I21:K25" si="3">C21/1000000000</f>
-        <v>4.6269999999999999E-6</v>
+        <f t="shared" ref="I21:K25" si="4">C21/1000000000</f>
+        <v>7.3799999999999996E-6</v>
       </c>
       <c r="J21" s="8">
-        <f t="shared" si="3"/>
-        <v>5.6330000000000001E-6</v>
+        <f t="shared" si="4"/>
+        <v>8.8189999999999998E-6</v>
       </c>
       <c r="K21" s="7">
-        <f t="shared" si="3"/>
-        <v>1.9888E-5</v>
-      </c>
-      <c r="L21" s="16">
+        <f t="shared" si="4"/>
+        <v>1.1198E-5</v>
+      </c>
+      <c r="L21" s="12">
         <f>I21/K21</f>
-        <v>0.23265285599356395</v>
-      </c>
-      <c r="M21" s="16">
+        <v>0.65904625826040364</v>
+      </c>
+      <c r="M21" s="12">
         <f>J21/K21</f>
-        <v>0.28323612228479483</v>
+        <v>0.78755134845508123</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="18">
-        <f t="shared" si="2"/>
-        <v>393779</v>
-      </c>
-      <c r="D22" s="18">
-        <f t="shared" si="2"/>
+      <c r="C22" s="14">
+        <f t="shared" si="3"/>
+        <v>382383</v>
+      </c>
+      <c r="D22" s="14">
+        <f t="shared" si="3"/>
         <v>607143</v>
       </c>
-      <c r="E22" s="18">
-        <f t="shared" si="2"/>
-        <v>32261</v>
+      <c r="E22" s="14">
+        <f t="shared" si="3"/>
+        <v>17909</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I22" s="7">
-        <f t="shared" si="3"/>
-        <v>3.9377900000000003E-4</v>
+        <f t="shared" si="4"/>
+        <v>3.8238299999999997E-4</v>
       </c>
       <c r="J22" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.0714299999999998E-4</v>
       </c>
       <c r="K22" s="8">
-        <f t="shared" si="3"/>
-        <v>3.2261000000000002E-5</v>
-      </c>
-      <c r="L22" s="16">
-        <f t="shared" ref="L22:L25" si="4">I22/K22</f>
-        <v>12.206038250519203</v>
-      </c>
-      <c r="M22" s="16">
-        <f t="shared" ref="M22:M25" si="5">J22/K22</f>
-        <v>18.819720405443103</v>
+        <f t="shared" si="4"/>
+        <v>1.7909000000000001E-5</v>
+      </c>
+      <c r="L22" s="12">
+        <f t="shared" ref="L22:L25" si="5">I22/K22</f>
+        <v>21.35144340834217</v>
+      </c>
+      <c r="M22" s="12">
+        <f t="shared" ref="M22:M25" si="6">J22/K22</f>
+        <v>33.901557875928304</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="14">
         <f>AVERAGE(C10:C14)</f>
-        <v>1479894.4</v>
-      </c>
-      <c r="D23" s="18">
+        <v>1445362.4</v>
+      </c>
+      <c r="D23" s="14">
         <f>AVERAGE(D10:D14)</f>
-        <v>2157995</v>
-      </c>
-      <c r="E23" s="18">
+        <v>2131435.6</v>
+      </c>
+      <c r="E23" s="14">
         <f>AVERAGE(E10:E14)</f>
-        <v>96714.8</v>
+        <v>88954.8</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I23" s="7">
-        <f t="shared" si="3"/>
-        <v>1.4798944E-3</v>
+        <f t="shared" si="4"/>
+        <v>1.4453623999999999E-3</v>
       </c>
       <c r="J23" s="7">
-        <f t="shared" si="3"/>
-        <v>2.1579949999999998E-3</v>
+        <f t="shared" si="4"/>
+        <v>2.1314356000000003E-3</v>
       </c>
       <c r="K23" s="8">
-        <f t="shared" si="3"/>
-        <v>9.6714799999999998E-5</v>
-      </c>
-      <c r="L23" s="16">
         <f t="shared" si="4"/>
-        <v>15.301633255716808</v>
-      </c>
-      <c r="M23" s="16">
+        <v>8.8954800000000004E-5</v>
+      </c>
+      <c r="L23" s="12">
         <f t="shared" si="5"/>
-        <v>22.312975883732374</v>
+        <v>16.248278901194762</v>
+      </c>
+      <c r="M23" s="12">
+        <f t="shared" si="6"/>
+        <v>23.960883504881132</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="14">
         <f>AVERAGE(C15:C18)</f>
-        <v>25353727.5</v>
-      </c>
-      <c r="D24" s="18">
+        <v>24884997</v>
+      </c>
+      <c r="D24" s="14">
         <f>AVERAGE(D15:D18)</f>
-        <v>17559434.5</v>
-      </c>
-      <c r="E24" s="18" t="s">
+        <v>17356671</v>
+      </c>
+      <c r="E24" s="14" t="s">
         <v>10</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I24" s="7">
-        <f t="shared" si="3"/>
-        <v>2.5353727499999999E-2</v>
+        <f t="shared" si="4"/>
+        <v>2.4884996999999999E-2</v>
       </c>
       <c r="J24" s="7">
-        <f t="shared" si="3"/>
-        <v>1.7559434499999999E-2</v>
+        <f t="shared" si="4"/>
+        <v>1.7356671000000001E-2</v>
       </c>
       <c r="K24" s="10" t="s">
         <v>10</v>
@@ -1194,63 +1199,46 @@
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="19">
+      <c r="B25" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="15">
         <f>AVERAGE(C8:C18)</f>
-        <v>9928435.2727272734</v>
-      </c>
-      <c r="D25" s="19">
+        <v>9741505.7272727266</v>
+      </c>
+      <c r="D25" s="15">
         <f>AVERAGE(D8:D18)</f>
-        <v>7421862.6363636367</v>
-      </c>
-      <c r="E25" s="19">
+        <v>7336347.6363636367</v>
+      </c>
+      <c r="E25" s="15">
         <f>AVERAGE(E8:E18)</f>
-        <v>76531.857142857145</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>19</v>
+        <v>67697.28571428571</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="I25" s="7">
-        <f t="shared" si="3"/>
-        <v>9.9284352727272741E-3</v>
+        <f t="shared" si="4"/>
+        <v>9.7415057272727274E-3</v>
       </c>
       <c r="J25" s="7">
-        <f t="shared" si="3"/>
-        <v>7.4218626363636367E-3</v>
-      </c>
-      <c r="K25" s="8">
-        <f t="shared" si="3"/>
-        <v>7.6531857142857142E-5</v>
-      </c>
-      <c r="L25" s="16">
         <f t="shared" si="4"/>
-        <v>129.72944396468122</v>
-      </c>
-      <c r="M25" s="16">
-        <f t="shared" si="5"/>
-        <v>96.977427615662307</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>16</v>
-      </c>
+        <v>7.3363476363636363E-3</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test results and readme corrected
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub.kolada\Documents\go_sudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BBB4F1-F5EA-42C8-B57A-E26183CC86FD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2BEB03-E446-4BF5-BBC5-3BD122014327}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{666A6699-6131-4AB1-A29E-7DACA2D9F716}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="21">
   <si>
     <t>Sudoku level</t>
   </si>
@@ -84,18 +84,26 @@
   </si>
   <si>
     <t>ALL LEVELS</t>
+  </si>
+  <si>
+    <t>Deduction in comparison to row backtracking</t>
+  </si>
+  <si>
+    <t>Backtracking by row [us]</t>
+  </si>
+  <si>
+    <t>µ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="#,##0.0000000"/>
-    <numFmt numFmtId="165" formatCode="0.0000000"/>
+  <numFmts count="2">
     <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +120,13 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -197,22 +212,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -222,6 +226,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -234,6 +239,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7BD8A7-F08D-41BA-B080-BFE118E322A3}">
-  <dimension ref="A5:M31"/>
+  <dimension ref="A5:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,71 +584,74 @@
     <col min="13" max="13" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="G5" s="19" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="G5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19" t="s">
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19" t="s">
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19" t="s">
+      <c r="J6" s="13"/>
+      <c r="K6" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
+      <c r="E7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
       <c r="I7" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="19"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K7" s="13"/>
+      <c r="L7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -642,13 +659,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>7380</v>
+        <v>7590</v>
       </c>
       <c r="D8" s="1">
-        <v>8819</v>
+        <v>8839</v>
       </c>
       <c r="E8" s="1">
-        <v>11198</v>
+        <v>12173</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>16</v>
@@ -657,20 +674,28 @@
         <f>B8</f>
         <v>1</v>
       </c>
-      <c r="I8" s="5">
-        <f>C8/1000000000</f>
-        <v>7.3799999999999996E-6</v>
-      </c>
-      <c r="J8" s="5">
-        <f t="shared" ref="J8:K18" si="0">D8/1000000000</f>
-        <v>8.8189999999999998E-6</v>
-      </c>
-      <c r="K8" s="6">
-        <f t="shared" si="0"/>
-        <v>1.1198E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I8" s="14">
+        <f>C8/1000</f>
+        <v>7.59</v>
+      </c>
+      <c r="J8" s="14">
+        <f>D8/1000</f>
+        <v>8.8390000000000004</v>
+      </c>
+      <c r="K8" s="14">
+        <f>E8/1000</f>
+        <v>12.173</v>
+      </c>
+      <c r="L8" s="9">
+        <f>(J8-K8)/J8</f>
+        <v>-0.37719199004412257</v>
+      </c>
+      <c r="M8" s="9">
+        <f>J8/K8</f>
+        <v>0.72611517292368355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -678,35 +703,43 @@
         <v>2</v>
       </c>
       <c r="C9" s="1">
-        <v>382383</v>
+        <v>379182</v>
       </c>
       <c r="D9" s="1">
-        <v>607143</v>
+        <v>572005</v>
       </c>
       <c r="E9" s="1">
-        <v>17909</v>
+        <v>19119</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" ref="H9:H18" si="1">B9</f>
+        <f t="shared" ref="H9:H18" si="0">B9</f>
         <v>2</v>
       </c>
-      <c r="I9" s="4">
-        <f t="shared" ref="I9:I18" si="2">C9/1000000000</f>
-        <v>3.8238299999999997E-4</v>
-      </c>
-      <c r="J9" s="4">
-        <f t="shared" si="0"/>
-        <v>6.0714299999999998E-4</v>
-      </c>
-      <c r="K9" s="5">
-        <f t="shared" si="0"/>
-        <v>1.7909000000000001E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I9" s="14">
+        <f t="shared" ref="I9:J18" si="1">C9/1000</f>
+        <v>379.18200000000002</v>
+      </c>
+      <c r="J9" s="14">
+        <f t="shared" ref="J9:J14" si="2">D9/1000</f>
+        <v>572.005</v>
+      </c>
+      <c r="K9" s="14">
+        <f t="shared" ref="K9:K14" si="3">E9/1000</f>
+        <v>19.119</v>
+      </c>
+      <c r="L9" s="9">
+        <f t="shared" ref="L9:L14" si="4">(J9-K9)/J9</f>
+        <v>0.96657546699766606</v>
+      </c>
+      <c r="M9" s="9">
+        <f t="shared" ref="M9:M14" si="5">J9/K9</f>
+        <v>29.918144254406613</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -714,35 +747,43 @@
         <v>3</v>
       </c>
       <c r="C10" s="1">
-        <v>161307</v>
+        <v>160607</v>
       </c>
       <c r="D10" s="1">
-        <v>221174</v>
+        <v>210879</v>
       </c>
       <c r="E10" s="1">
-        <v>37858</v>
+        <v>39510</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H10" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I10" s="14">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I10" s="4">
+        <v>160.607</v>
+      </c>
+      <c r="J10" s="14">
         <f t="shared" si="2"/>
-        <v>1.6130699999999999E-4</v>
-      </c>
-      <c r="J10" s="4">
-        <f t="shared" si="0"/>
-        <v>2.2117400000000001E-4</v>
-      </c>
-      <c r="K10" s="5">
-        <f t="shared" si="0"/>
-        <v>3.7858000000000002E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>210.87899999999999</v>
+      </c>
+      <c r="K10" s="14">
+        <f t="shared" si="3"/>
+        <v>39.51</v>
+      </c>
+      <c r="L10" s="9">
+        <f t="shared" si="4"/>
+        <v>0.81264137254065127</v>
+      </c>
+      <c r="M10" s="9">
+        <f t="shared" si="5"/>
+        <v>5.3373576309794988</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -750,35 +791,43 @@
         <v>4</v>
       </c>
       <c r="C11" s="1">
-        <v>632639</v>
+        <v>634629</v>
       </c>
       <c r="D11" s="1">
-        <v>798050</v>
-      </c>
-      <c r="E11" s="11">
-        <v>106140</v>
+        <v>759564</v>
+      </c>
+      <c r="E11" s="4">
+        <v>114236</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I11" s="14">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="I11" s="4">
+        <v>634.62900000000002</v>
+      </c>
+      <c r="J11" s="14">
         <f t="shared" si="2"/>
-        <v>6.3263900000000005E-4</v>
-      </c>
-      <c r="J11" s="4">
-        <f t="shared" si="0"/>
-        <v>7.9805000000000002E-4</v>
-      </c>
-      <c r="K11" s="5">
-        <f t="shared" si="0"/>
-        <v>1.0614E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>759.56399999999996</v>
+      </c>
+      <c r="K11" s="14">
+        <f t="shared" si="3"/>
+        <v>114.236</v>
+      </c>
+      <c r="L11" s="9">
+        <f t="shared" si="4"/>
+        <v>0.8496031934109568</v>
+      </c>
+      <c r="M11" s="9">
+        <f t="shared" si="5"/>
+        <v>6.649077348646661</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -789,32 +838,40 @@
         <v>275644</v>
       </c>
       <c r="D12" s="1">
-        <v>306227</v>
+        <v>294231</v>
       </c>
       <c r="E12" s="1">
-        <v>81753</v>
+        <v>71358</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H12" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I12" s="14">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="I12" s="4">
+        <v>275.64400000000001</v>
+      </c>
+      <c r="J12" s="14">
         <f t="shared" si="2"/>
-        <v>2.7564400000000002E-4</v>
-      </c>
-      <c r="J12" s="4">
-        <f t="shared" si="0"/>
-        <v>3.0622700000000001E-4</v>
-      </c>
-      <c r="K12" s="5">
-        <f t="shared" si="0"/>
-        <v>8.1753000000000001E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>294.23099999999999</v>
+      </c>
+      <c r="K12" s="14">
+        <f t="shared" si="3"/>
+        <v>71.358000000000004</v>
+      </c>
+      <c r="L12" s="9">
+        <f t="shared" si="4"/>
+        <v>0.75747626864606377</v>
+      </c>
+      <c r="M12" s="9">
+        <f t="shared" si="5"/>
+        <v>4.1233078281341964</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -822,35 +879,43 @@
         <v>6</v>
       </c>
       <c r="C13" s="1">
-        <v>360593</v>
+        <v>362789</v>
       </c>
       <c r="D13" s="1">
         <v>216975</v>
       </c>
       <c r="E13" s="1">
-        <v>138219</v>
+        <v>123229</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I13" s="14">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="I13" s="4">
+        <v>362.78899999999999</v>
+      </c>
+      <c r="J13" s="14">
         <f t="shared" si="2"/>
-        <v>3.6059299999999998E-4</v>
-      </c>
-      <c r="J13" s="4">
-        <f t="shared" si="0"/>
-        <v>2.16975E-4</v>
-      </c>
-      <c r="K13" s="5">
-        <f t="shared" si="0"/>
-        <v>1.38219E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>216.97499999999999</v>
+      </c>
+      <c r="K13" s="14">
+        <f t="shared" si="3"/>
+        <v>123.229</v>
+      </c>
+      <c r="L13" s="9">
+        <f t="shared" si="4"/>
+        <v>0.43205899297154049</v>
+      </c>
+      <c r="M13" s="9">
+        <f t="shared" si="5"/>
+        <v>1.7607462529112465</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -858,35 +923,43 @@
         <v>7</v>
       </c>
       <c r="C14" s="1">
-        <v>5796629</v>
+        <v>6321463</v>
       </c>
       <c r="D14" s="1">
-        <v>9114752</v>
+        <v>8804953</v>
       </c>
       <c r="E14" s="1">
-        <v>80804</v>
+        <v>108337</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H14" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I14" s="14">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="I14" s="4">
-        <f t="shared" si="2"/>
-        <v>5.7966290000000002E-3</v>
-      </c>
-      <c r="J14" s="4">
-        <f t="shared" si="0"/>
-        <v>9.1147520000000003E-3</v>
-      </c>
-      <c r="K14" s="5">
-        <f t="shared" si="0"/>
-        <v>8.0803999999999994E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+        <v>6321.4629999999997</v>
+      </c>
+      <c r="J14" s="14">
+        <f t="shared" si="1"/>
+        <v>8804.9529999999995</v>
+      </c>
+      <c r="K14" s="14">
+        <f t="shared" si="3"/>
+        <v>108.337</v>
+      </c>
+      <c r="L14" s="9">
+        <f t="shared" si="4"/>
+        <v>0.98769590252213735</v>
+      </c>
+      <c r="M14" s="9">
+        <f t="shared" si="5"/>
+        <v>81.273738427314754</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -894,10 +967,10 @@
         <v>8</v>
       </c>
       <c r="C15" s="1">
-        <v>86150620</v>
+        <v>87149385</v>
       </c>
       <c r="D15" s="1">
-        <v>47439333</v>
+        <v>46973070</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>10</v>
@@ -906,22 +979,22 @@
         <v>4</v>
       </c>
       <c r="H15" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I15" s="14">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="I15" s="4">
-        <f t="shared" si="2"/>
-        <v>8.6150619999999997E-2</v>
-      </c>
-      <c r="J15" s="4">
-        <f t="shared" si="0"/>
-        <v>4.7439333E-2</v>
-      </c>
-      <c r="K15" s="9" t="s">
+        <v>87149.384999999995</v>
+      </c>
+      <c r="J15" s="14">
+        <f t="shared" si="1"/>
+        <v>46973.07</v>
+      </c>
+      <c r="K15" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -929,10 +1002,10 @@
         <v>9</v>
       </c>
       <c r="C16" s="1">
-        <v>3336116</v>
+        <v>3398052</v>
       </c>
       <c r="D16" s="1">
-        <v>1257266</v>
+        <v>1359221</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>10</v>
@@ -941,18 +1014,18 @@
         <v>4</v>
       </c>
       <c r="H16" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I16" s="14">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="I16" s="4">
-        <f t="shared" si="2"/>
-        <v>3.3361160000000001E-3</v>
-      </c>
-      <c r="J16" s="4">
-        <f t="shared" si="0"/>
-        <v>1.2572659999999999E-3</v>
-      </c>
-      <c r="K16" s="9" t="s">
+        <v>3398.0520000000001</v>
+      </c>
+      <c r="J16" s="14">
+        <f t="shared" si="1"/>
+        <v>1359.221</v>
+      </c>
+      <c r="K16" s="15" t="s">
         <v>10</v>
       </c>
     </row>
@@ -964,10 +1037,10 @@
         <v>10</v>
       </c>
       <c r="C17" s="1">
-        <v>2097809</v>
+        <v>2186746</v>
       </c>
       <c r="D17" s="1">
-        <v>1611088</v>
+        <v>1624070</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>10</v>
@@ -976,18 +1049,18 @@
         <v>4</v>
       </c>
       <c r="H17" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I17" s="14">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="I17" s="4">
-        <f t="shared" si="2"/>
-        <v>2.097809E-3</v>
-      </c>
-      <c r="J17" s="4">
-        <f t="shared" si="0"/>
-        <v>1.6110880000000001E-3</v>
-      </c>
-      <c r="K17" s="9" t="s">
+        <v>2186.7460000000001</v>
+      </c>
+      <c r="J17" s="14">
+        <f t="shared" si="1"/>
+        <v>1624.07</v>
+      </c>
+      <c r="K17" s="15" t="s">
         <v>10</v>
       </c>
     </row>
@@ -999,10 +1072,10 @@
         <v>11</v>
       </c>
       <c r="C18" s="1">
-        <v>7955443</v>
+        <v>8355282</v>
       </c>
       <c r="D18" s="1">
-        <v>19118997</v>
+        <v>19648719</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>10</v>
@@ -1011,34 +1084,34 @@
         <v>5</v>
       </c>
       <c r="H18" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="I18" s="14">
         <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="I18" s="4">
-        <f t="shared" si="2"/>
-        <v>7.9554429999999995E-3</v>
-      </c>
-      <c r="J18" s="4">
-        <f t="shared" si="0"/>
-        <v>1.9118996999999999E-2</v>
-      </c>
-      <c r="K18" s="9" t="s">
+        <v>8355.2819999999992</v>
+      </c>
+      <c r="J18" s="14">
+        <f t="shared" si="1"/>
+        <v>19648.719000000001</v>
+      </c>
+      <c r="K18" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18"/>
-      <c r="H20" s="16" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="H20" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="18"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="12"/>
       <c r="L20" s="1" t="s">
         <v>15</v>
       </c>
@@ -1051,185 +1124,185 @@
         <v>16</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" ref="C21:E22" si="3">AVERAGE(C8)</f>
-        <v>7380</v>
+        <f t="shared" ref="C21:E22" si="6">AVERAGE(C8)</f>
+        <v>7590</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="3"/>
-        <v>8819</v>
+        <f t="shared" si="6"/>
+        <v>8839</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="3"/>
-        <v>11198</v>
+        <f t="shared" si="6"/>
+        <v>12173</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="8">
-        <f t="shared" ref="I21:K25" si="4">C21/1000000000</f>
-        <v>7.3799999999999996E-6</v>
-      </c>
-      <c r="J21" s="8">
-        <f t="shared" si="4"/>
-        <v>8.8189999999999998E-6</v>
-      </c>
-      <c r="K21" s="7">
-        <f t="shared" si="4"/>
-        <v>1.1198E-5</v>
-      </c>
-      <c r="L21" s="12">
+      <c r="I21" s="16">
+        <f>C21/1000</f>
+        <v>7.59</v>
+      </c>
+      <c r="J21" s="16">
+        <f t="shared" ref="J21:K23" si="7">D21/1000</f>
+        <v>8.8390000000000004</v>
+      </c>
+      <c r="K21" s="16">
+        <f t="shared" si="7"/>
+        <v>12.173</v>
+      </c>
+      <c r="L21" s="5">
         <f>I21/K21</f>
-        <v>0.65904625826040364</v>
-      </c>
-      <c r="M21" s="12">
+        <v>0.62351104904296395</v>
+      </c>
+      <c r="M21" s="5">
         <f>J21/K21</f>
-        <v>0.78755134845508123</v>
+        <v>0.72611517292368355</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="14">
-        <f t="shared" si="3"/>
-        <v>382383</v>
-      </c>
-      <c r="D22" s="14">
-        <f t="shared" si="3"/>
-        <v>607143</v>
-      </c>
-      <c r="E22" s="14">
-        <f t="shared" si="3"/>
-        <v>17909</v>
+      <c r="C22" s="7">
+        <f t="shared" si="6"/>
+        <v>379182</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="6"/>
+        <v>572005</v>
+      </c>
+      <c r="E22" s="7">
+        <f t="shared" si="6"/>
+        <v>19119</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I22" s="7">
-        <f t="shared" si="4"/>
-        <v>3.8238299999999997E-4</v>
-      </c>
-      <c r="J22" s="7">
-        <f t="shared" si="4"/>
-        <v>6.0714299999999998E-4</v>
-      </c>
-      <c r="K22" s="8">
-        <f t="shared" si="4"/>
-        <v>1.7909000000000001E-5</v>
-      </c>
-      <c r="L22" s="12">
-        <f t="shared" ref="L22:L25" si="5">I22/K22</f>
-        <v>21.35144340834217</v>
-      </c>
-      <c r="M22" s="12">
-        <f t="shared" ref="M22:M25" si="6">J22/K22</f>
-        <v>33.901557875928304</v>
+      <c r="I22" s="16">
+        <f t="shared" ref="I22:J25" si="8">C22/1000</f>
+        <v>379.18200000000002</v>
+      </c>
+      <c r="J22" s="16">
+        <f t="shared" si="7"/>
+        <v>572.005</v>
+      </c>
+      <c r="K22" s="16">
+        <f t="shared" si="7"/>
+        <v>19.119</v>
+      </c>
+      <c r="L22" s="5">
+        <f t="shared" ref="L22:L23" si="9">I22/K22</f>
+        <v>19.832731837439198</v>
+      </c>
+      <c r="M22" s="5">
+        <f t="shared" ref="M22:M23" si="10">J22/K22</f>
+        <v>29.918144254406613</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="7">
         <f>AVERAGE(C10:C14)</f>
-        <v>1445362.4</v>
-      </c>
-      <c r="D23" s="14">
+        <v>1551026.4</v>
+      </c>
+      <c r="D23" s="7">
         <f>AVERAGE(D10:D14)</f>
-        <v>2131435.6</v>
-      </c>
-      <c r="E23" s="14">
+        <v>2057320.4</v>
+      </c>
+      <c r="E23" s="7">
         <f>AVERAGE(E10:E14)</f>
-        <v>88954.8</v>
+        <v>91334</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I23" s="7">
-        <f t="shared" si="4"/>
-        <v>1.4453623999999999E-3</v>
-      </c>
-      <c r="J23" s="7">
-        <f t="shared" si="4"/>
-        <v>2.1314356000000003E-3</v>
-      </c>
-      <c r="K23" s="8">
-        <f t="shared" si="4"/>
-        <v>8.8954800000000004E-5</v>
-      </c>
-      <c r="L23" s="12">
-        <f t="shared" si="5"/>
-        <v>16.248278901194762</v>
-      </c>
-      <c r="M23" s="12">
-        <f t="shared" si="6"/>
-        <v>23.960883504881132</v>
+      <c r="I23" s="16">
+        <f t="shared" si="8"/>
+        <v>1551.0264</v>
+      </c>
+      <c r="J23" s="16">
+        <f t="shared" si="7"/>
+        <v>2057.3204000000001</v>
+      </c>
+      <c r="K23" s="16">
+        <f t="shared" si="7"/>
+        <v>91.334000000000003</v>
+      </c>
+      <c r="L23" s="5">
+        <f t="shared" si="9"/>
+        <v>16.98191692031445</v>
+      </c>
+      <c r="M23" s="5">
+        <f t="shared" si="10"/>
+        <v>22.525241421595464</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="7">
         <f>AVERAGE(C15:C18)</f>
-        <v>24884997</v>
-      </c>
-      <c r="D24" s="14">
+        <v>25272366.25</v>
+      </c>
+      <c r="D24" s="7">
         <f>AVERAGE(D15:D18)</f>
-        <v>17356671</v>
-      </c>
-      <c r="E24" s="14" t="s">
+        <v>17401270</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>10</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="7">
-        <f t="shared" si="4"/>
-        <v>2.4884996999999999E-2</v>
-      </c>
-      <c r="J24" s="7">
-        <f t="shared" si="4"/>
-        <v>1.7356671000000001E-2</v>
-      </c>
-      <c r="K24" s="10" t="s">
+      <c r="I24" s="16">
+        <f t="shared" si="8"/>
+        <v>25272.366249999999</v>
+      </c>
+      <c r="J24" s="16">
+        <f t="shared" si="8"/>
+        <v>17401.27</v>
+      </c>
+      <c r="K24" s="17" t="s">
         <v>10</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="8">
         <f>AVERAGE(C8:C18)</f>
-        <v>9741505.7272727266</v>
-      </c>
-      <c r="D25" s="15">
+        <v>9930124.4545454551</v>
+      </c>
+      <c r="D25" s="8">
         <f>AVERAGE(D8:D18)</f>
-        <v>7336347.6363636367</v>
-      </c>
-      <c r="E25" s="15">
+        <v>7315684.1818181816</v>
+      </c>
+      <c r="E25" s="8">
         <f>AVERAGE(E8:E18)</f>
-        <v>67697.28571428571</v>
-      </c>
-      <c r="H25" s="13" t="s">
+        <v>69708.857142857145</v>
+      </c>
+      <c r="H25" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I25" s="7">
-        <f t="shared" si="4"/>
-        <v>9.7415057272727274E-3</v>
-      </c>
-      <c r="J25" s="7">
-        <f t="shared" si="4"/>
-        <v>7.3363476363636363E-3</v>
-      </c>
-      <c r="K25" s="10" t="s">
+      <c r="I25" s="16">
+        <f t="shared" si="8"/>
+        <v>9930.1244545454556</v>
+      </c>
+      <c r="J25" s="16">
+        <f t="shared" si="8"/>
+        <v>7315.684181818182</v>
+      </c>
+      <c r="K25" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -1239,6 +1312,11 @@
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J36" s="18" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>